<commit_message>
Bug fixed for estimate and output intervals
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1237570423861605</v>
+        <v>-0.5756590284122012</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04711888429185662</v>
+        <v>0.3207495939781946</v>
       </c>
       <c r="D2" t="n">
-        <v>0.202367195458658</v>
+        <v>1.95978415313909</v>
       </c>
       <c r="E2" t="n">
-        <v>1.785937648078703</v>
+        <v>2.39621060139114</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.3034824872474815</v>
+        <v>-0.291008655205852</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.6662433246155821</v>
+        <v>-0.2264202648008908</v>
       </c>
       <c r="D3" t="n">
-        <v>4.185028280186422</v>
+        <v>1.276839481418494</v>
       </c>
       <c r="E3" t="n">
-        <v>3.744228957961562</v>
+        <v>1.155356738246432</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4748318035931334</v>
+        <v>-0.5647922974256379</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.6499983815204486</v>
+        <v>-0.8134551205460301</v>
       </c>
       <c r="D4" t="n">
-        <v>5.991119170253434</v>
+        <v>9.642744040232234</v>
       </c>
       <c r="E4" t="n">
-        <v>8.056009862856136</v>
+        <v>10.21182065410205</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2414643987679537</v>
+        <v>0.4807540316317152</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.397707659234495</v>
+        <v>-0.4759676014471899</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4672771001722301</v>
+        <v>1.716234575219484</v>
       </c>
       <c r="E5" t="n">
-        <v>5.322836508827448</v>
+        <v>3.054409674085557</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.9873850224539116</v>
+        <v>-0.6634324583168609</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3598864094325809</v>
+        <v>-0.2754514985501237</v>
       </c>
       <c r="D6" t="n">
-        <v>12.10387247791295</v>
+        <v>5.557882352601584</v>
       </c>
       <c r="E6" t="n">
-        <v>11.35736996062962</v>
+        <v>5.352148883850542</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.8875403975732277</v>
+        <v>0.3618879371679125</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3636095754509796</v>
+        <v>-0.07323553105339564</v>
       </c>
       <c r="D7" t="n">
-        <v>5.547103432395954</v>
+        <v>1.182761606206032</v>
       </c>
       <c r="E7" t="n">
-        <v>4.800653256488223</v>
+        <v>0.9770425625540523</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.05651750129072464</v>
+        <v>-0.948465924889776</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.6442028007756828</v>
+        <v>0.2709656372022857</v>
       </c>
       <c r="D8" t="n">
-        <v>2.125429238660431</v>
+        <v>7.254193686124503</v>
       </c>
       <c r="E8" t="n">
-        <v>7.160105093728854</v>
+        <v>8.641732647774393</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6077882087480229</v>
+        <v>-0.6332185671412767</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.4236710971620972</v>
+        <v>0.3693039979341373</v>
       </c>
       <c r="D9" t="n">
-        <v>2.7389306947416</v>
+        <v>2.241229909388999</v>
       </c>
       <c r="E9" t="n">
-        <v>5.185583269534513</v>
+        <v>2.915518755557438</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.02033783740578565</v>
+        <v>0.8346960447089338</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.2013052737689545</v>
+        <v>0.1634371366947018</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07775789499939399</v>
+        <v>7.857621564116275</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.41896967219702</v>
+        <v>7.445128709711399</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.7956392543679587</v>
+        <v>-0.1336843864950779</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8203215729205784</v>
+        <v>-0.6731292637382853</v>
       </c>
       <c r="D11" t="n">
-        <v>6.57025273181165</v>
+        <v>2.818243571775921</v>
       </c>
       <c r="E11" t="n">
-        <v>8.299984104647221</v>
+        <v>3.294951455676997</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.498626635975101</v>
+        <v>0.6303452495428949</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4987675433707282</v>
+        <v>0.2475570504516955</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1254996085742737</v>
+        <v>4.897348621319452</v>
       </c>
       <c r="E12" t="n">
-        <v>-1.351918663303662</v>
+        <v>4.490177340804864</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1028510711828035</v>
+        <v>-0.7562929567815557</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.9854877926993884</v>
+        <v>-0.8334758938977451</v>
       </c>
       <c r="D13" t="n">
-        <v>6.255406853917449</v>
+        <v>13.46539866532799</v>
       </c>
       <c r="E13" t="n">
-        <v>4.770617519470609</v>
+        <v>13.05619594588912</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.6048896830170214</v>
+        <v>-0.4357068012813932</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3265627374653448</v>
+        <v>-0.3695531090647688</v>
       </c>
       <c r="D14" t="n">
-        <v>2.196432276004371</v>
+        <v>3.150923728545163</v>
       </c>
       <c r="E14" t="n">
-        <v>2.967830275392832</v>
+        <v>3.363518304621546</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.08380279640401533</v>
+        <v>-0.5864834637815606</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.527682844767434</v>
+        <v>-0.4139342885863653</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8432723598826919</v>
+        <v>5.309783738666794</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.25644121713959</v>
+        <v>3.628724125960463</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.4576369515978949</v>
+        <v>0.4409109498032153</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4592864190506201</v>
+        <v>-0.141025519633132</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1533061535951519</v>
+        <v>1.62255704785273</v>
       </c>
       <c r="E16" t="n">
-        <v>-5.345890710850302</v>
+        <v>0.1069977294669229</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.42867712555207</v>
+        <v>0.07823337889928728</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8630103946599155</v>
+        <v>-0.8722598223474136</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.2814575070286786</v>
+        <v>4.293980724276393</v>
       </c>
       <c r="E17" t="n">
-        <v>-2.074081920455847</v>
+        <v>3.79993973954627</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2536544366700308</v>
+        <v>0.9670863720555543</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.3897815655848755</v>
+        <v>-0.2294394079850954</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4857918133779077</v>
+        <v>8.184810857696846</v>
       </c>
       <c r="E18" t="n">
-        <v>-2.74320705031942</v>
+        <v>7.29491012536015</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.4226729074551507</v>
+        <v>-0.05517337373057218</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.7590394561584064</v>
+        <v>0.3716164230887973</v>
       </c>
       <c r="D19" t="n">
-        <v>6.750066882479985</v>
+        <v>-0.4063631834994618</v>
       </c>
       <c r="E19" t="n">
-        <v>7.751916311765899</v>
+        <v>-0.1302570037060815</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4113420081781205</v>
+        <v>-0.5241259994243446</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.3758961630445221</v>
+        <v>-0.05435091973715567</v>
       </c>
       <c r="D20" t="n">
-        <v>2.945747991934274</v>
+        <v>2.861572600687941</v>
       </c>
       <c r="E20" t="n">
-        <v>0.05088363675954843</v>
+        <v>2.063758163944658</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.7134379102518238</v>
+        <v>-0.1157366431678277</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9202244262435784</v>
+        <v>-0.5493427286363373</v>
       </c>
       <c r="D21" t="n">
-        <v>-4.244658717130096</v>
+        <v>1.639548683393787</v>
       </c>
       <c r="E21" t="n">
-        <v>-8.74721294877873</v>
+        <v>0.3986605699982206</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.6539634487664148</v>
+        <v>0.2963567303404737</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6122949999871423</v>
+        <v>-0.5280645993584079</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2700116313203534</v>
+        <v>0.9747784678334531</v>
       </c>
       <c r="E22" t="n">
-        <v>4.942634849951756</v>
+        <v>2.262536996008426</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.7331742559103274</v>
+        <v>0.2952347051379052</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7814213856360559</v>
+        <v>-0.4223396496351903</v>
       </c>
       <c r="D23" t="n">
-        <v>-1.375305085280847</v>
+        <v>0.6559573312152873</v>
       </c>
       <c r="E23" t="n">
-        <v>-2.095100718614164</v>
+        <v>0.4575841857683967</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1833453374036449</v>
+        <v>0.7666815627295551</v>
       </c>
       <c r="C24" t="n">
-        <v>0.09862020907608371</v>
+        <v>0.8112092597798641</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4621683757356684</v>
+        <v>6.096463224361921</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6774545096499085</v>
+        <v>6.155795325833412</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.07049386628820242</v>
+        <v>0.2268149571524618</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8671411406609306</v>
+        <v>0.2160857437047459</v>
       </c>
       <c r="D25" t="n">
-        <v>-4.022166414219738</v>
+        <v>0.7868505800505254</v>
       </c>
       <c r="E25" t="n">
-        <v>-8.564394809432407</v>
+        <v>-0.4649715933124869</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8847403553876032</v>
+        <v>-0.4058460379469071</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01384084700390042</v>
+        <v>0.9111246494296348</v>
       </c>
       <c r="D26" t="n">
-        <v>7.990294974344962</v>
+        <v>-5.732584182306792</v>
       </c>
       <c r="E26" t="n">
-        <v>6.254752726859651</v>
+        <v>-6.210893522827893</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.9532733727010809</v>
+        <v>0.7310479976046806</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.8452565451717211</v>
+        <v>0.0878981715760645</v>
       </c>
       <c r="D27" t="n">
-        <v>8.604554074058878</v>
+        <v>5.807771904326657</v>
       </c>
       <c r="E27" t="n">
-        <v>8.958185502774516</v>
+        <v>5.905231482566018</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.7861909513031973</v>
+        <v>-0.6440375030485301</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.1606036239366995</v>
+        <v>0.1000887582096024</v>
       </c>
       <c r="D28" t="n">
-        <v>5.52553742415647</v>
+        <v>3.70066581550196</v>
       </c>
       <c r="E28" t="n">
-        <v>1.856063926548716</v>
+        <v>2.689371822950923</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.3225589924596985</v>
+        <v>-0.184847749655817</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.7814178533552936</v>
+        <v>-0.7305885748617531</v>
       </c>
       <c r="D29" t="n">
-        <v>5.882509773624601</v>
+        <v>3.843516158044857</v>
       </c>
       <c r="E29" t="n">
-        <v>7.080269646890494</v>
+        <v>4.173614567296802</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.2649097964361804</v>
+        <v>-0.4758370104471834</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.7928951492215366</v>
+        <v>-0.07207107833284199</v>
       </c>
       <c r="D30" t="n">
-        <v>5.448135033211742</v>
+        <v>2.418322220502919</v>
       </c>
       <c r="E30" t="n">
-        <v>3.533243588525399</v>
+        <v>1.890584871899324</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.2537827062456279</v>
+        <v>0.08866547626951493</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6084183608437965</v>
+        <v>-0.3345651838972654</v>
       </c>
       <c r="D31" t="n">
-        <v>-1.816859722418558</v>
+        <v>0.1493770065625539</v>
       </c>
       <c r="E31" t="n">
-        <v>-2.746806253207528</v>
+        <v>-0.1069129872454604</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.9958370723291672</v>
+        <v>0.5608069931705819</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.4088279877511498</v>
+        <v>0.3219429059760415</v>
       </c>
       <c r="D32" t="n">
-        <v>8.048336183100059</v>
+        <v>4.093392104145329</v>
       </c>
       <c r="E32" t="n">
-        <v>6.130040103763192</v>
+        <v>3.564716450204156</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.07230880414828111</v>
+        <v>-0.5951892846955613</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.429668017553648</v>
+        <v>0.09286154297029192</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4253428287815494</v>
+        <v>3.155905837981347</v>
       </c>
       <c r="E33" t="n">
-        <v>6.33057622154683</v>
+        <v>4.783367395779379</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.7929939285218528</v>
+        <v>0.4538544697719169</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.1010868920509123</v>
+        <v>-0.1522732820585742</v>
       </c>
       <c r="D34" t="n">
-        <v>5.889923598172865</v>
+        <v>1.702371659812536</v>
       </c>
       <c r="E34" t="n">
-        <v>5.846893203009389</v>
+        <v>1.690512634218186</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.3647250139316267</v>
+        <v>-0.5306171011841785</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.3434530324466321</v>
+        <v>-0.2095438448318574</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8933397370146448</v>
+        <v>3.477450605130413</v>
       </c>
       <c r="E35" t="n">
-        <v>-2.478740088683388</v>
+        <v>2.548117262798288</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.7018169062335478</v>
+        <v>0.9423664686105293</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.3084731336293922</v>
+        <v>-0.9972931390218613</v>
       </c>
       <c r="D36" t="n">
-        <v>6.353800663623576</v>
+        <v>10.27892827319895</v>
       </c>
       <c r="E36" t="n">
-        <v>8.976149575695157</v>
+        <v>11.00163841210025</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.9796489945014246</v>
+        <v>0.5998226843723065</v>
       </c>
       <c r="C37" t="n">
-        <v>0.094112751159799</v>
+        <v>-0.2767790327786326</v>
       </c>
       <c r="D37" t="n">
-        <v>10.24802751977914</v>
+        <v>2.790149269294258</v>
       </c>
       <c r="E37" t="n">
-        <v>6.355865559740933</v>
+        <v>1.717483119562315</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.2955996181486389</v>
+        <v>-0.7278056394991492</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.762599878955704</v>
+        <v>-0.173631268894324</v>
       </c>
       <c r="D38" t="n">
-        <v>2.67530726413504</v>
+        <v>6.004742706644631</v>
       </c>
       <c r="E38" t="n">
-        <v>3.341183635227793</v>
+        <v>6.188255893020496</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.4260704503355819</v>
+        <v>0.4895541461123263</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2373890531221061</v>
+        <v>0.7032373495384228</v>
       </c>
       <c r="D39" t="n">
-        <v>1.089747253793916</v>
+        <v>2.196535980703794</v>
       </c>
       <c r="E39" t="n">
-        <v>-5.157861529336727</v>
+        <v>0.4747169692548396</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.02170792273792377</v>
+        <v>-0.07620693659562239</v>
       </c>
       <c r="C40" t="n">
-        <v>0.7431865760356628</v>
+        <v>0.5177376255527129</v>
       </c>
       <c r="D40" t="n">
-        <v>-2.677297064101507</v>
+        <v>-1.079163068915913</v>
       </c>
       <c r="E40" t="n">
-        <v>-6.911676475010206</v>
+        <v>-2.246143144729371</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.3485752534519384</v>
+        <v>0.7947165474535383</v>
       </c>
       <c r="C41" t="n">
-        <v>0.5741890870038595</v>
+        <v>0.5605958724618121</v>
       </c>
       <c r="D41" t="n">
-        <v>-1.284163617479113</v>
+        <v>7.922550466137658</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.6565518723763725</v>
+        <v>8.095518056144959</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.09744845136867664</v>
+        <v>-0.1833657298573153</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0318875734491213</v>
+        <v>0.3531076731724552</v>
       </c>
       <c r="D42" t="n">
-        <v>0.06804188724463753</v>
+        <v>-0.3310051541037327</v>
       </c>
       <c r="E42" t="n">
-        <v>2.422341335405648</v>
+        <v>0.3178314951168243</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.5293887648163724</v>
+        <v>0.4491961500955992</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.8212893585856538</v>
+        <v>0.8615938481000833</v>
       </c>
       <c r="D43" t="n">
-        <v>4.150973419441931</v>
+        <v>0.0680401271640044</v>
       </c>
       <c r="E43" t="n">
-        <v>4.697311277873324</v>
+        <v>0.2186089197973524</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.8570942557180488</v>
+        <v>0.1011533271987117</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.4359937604181678</v>
+        <v>-0.8724131151366339</v>
       </c>
       <c r="D44" t="n">
-        <v>5.767046023658033</v>
+        <v>4.219803216494925</v>
       </c>
       <c r="E44" t="n">
-        <v>5.3983486515859</v>
+        <v>4.118191517244615</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.3037402229995689</v>
+        <v>-0.7665941407097365</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.1667895702086346</v>
+        <v>0.6753467061942988</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6759125970675041</v>
+        <v>0.6507022147076265</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.2840337072994575</v>
+        <v>0.3861443887931552</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.8096594315422618</v>
+        <v>-0.4337857442767545</v>
       </c>
       <c r="C46" t="n">
-        <v>0.9221869738428725</v>
+        <v>0.5644922107675316</v>
       </c>
       <c r="D46" t="n">
-        <v>5.757765784432831</v>
+        <v>-0.8017093851893232</v>
       </c>
       <c r="E46" t="n">
-        <v>1.044101550585462</v>
+        <v>-2.100778672840597</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.434253257950453</v>
+        <v>0.4124054653352369</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2989206365350809</v>
+        <v>-0.5125844158942694</v>
       </c>
       <c r="D47" t="n">
-        <v>2.544941860516688</v>
+        <v>1.39142836748686</v>
       </c>
       <c r="E47" t="n">
-        <v>0.2500122475935211</v>
+        <v>0.7589538360889054</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.7489117746757532</v>
+        <v>0.8626089339445611</v>
       </c>
       <c r="C48" t="n">
-        <v>0.8912525898594397</v>
+        <v>0.8021637960404688</v>
       </c>
       <c r="D48" t="n">
-        <v>-3.30267236313707</v>
+        <v>8.210327471960502</v>
       </c>
       <c r="E48" t="n">
-        <v>-4.771231176291395</v>
+        <v>7.805597827116612</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.4193159684754257</v>
+        <v>-0.5012539879044589</v>
       </c>
       <c r="C49" t="n">
-        <v>0.9221456908833179</v>
+        <v>0.681770485109749</v>
       </c>
       <c r="D49" t="n">
-        <v>-5.961596097548318</v>
+        <v>-1.691613613718977</v>
       </c>
       <c r="E49" t="n">
-        <v>-2.591393110378066</v>
+        <v>-0.7627975214853652</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.2734359437516378</v>
+        <v>0.3062833262166038</v>
       </c>
       <c r="C50" t="n">
-        <v>0.01355640823453919</v>
+        <v>-0.0428540728917024</v>
       </c>
       <c r="D50" t="n">
-        <v>0.6987664619167739</v>
+        <v>0.8864193057523926</v>
       </c>
       <c r="E50" t="n">
-        <v>1.794253206237806</v>
+        <v>1.188331600301843</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.66247570801372</v>
+        <v>0.6479863097144785</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.9597949941359096</v>
+        <v>-0.7930093530862083</v>
       </c>
       <c r="D51" t="n">
-        <v>6.873259137245841</v>
+        <v>4.654955744906443</v>
       </c>
       <c r="E51" t="n">
-        <v>1.252524797606553</v>
+        <v>3.105901125733351</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.7839929695697814</v>
+        <v>0.1082014294102274</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.4112381044126574</v>
+        <v>-0.9301912299238184</v>
       </c>
       <c r="D52" t="n">
-        <v>8.4856777790585</v>
+        <v>5.151486965642409</v>
       </c>
       <c r="E52" t="n">
-        <v>9.518887312127333</v>
+        <v>5.436235879763239</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.2603544488914127</v>
+        <v>0.8389288127753052</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.490480593079496</v>
+        <v>-0.2499726890171396</v>
       </c>
       <c r="D53" t="n">
-        <v>2.24350344009147</v>
+        <v>5.954243186857469</v>
       </c>
       <c r="E53" t="n">
-        <v>1.015825675328774</v>
+        <v>5.615899511912712</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.6346294530845378</v>
+        <v>0.6241782753952152</v>
       </c>
       <c r="C54" t="n">
-        <v>0.5759497600544075</v>
+        <v>0.1011661416385252</v>
       </c>
       <c r="D54" t="n">
-        <v>0.4955928692056598</v>
+        <v>4.341169585570059</v>
       </c>
       <c r="E54" t="n">
-        <v>-1.662496792452787</v>
+        <v>3.746407663554678</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.4324311363844608</v>
+        <v>-0.2095804160638219</v>
       </c>
       <c r="C55" t="n">
-        <v>0.3959827842266361</v>
+        <v>-0.8325706949567806</v>
       </c>
       <c r="D55" t="n">
-        <v>2.541463818186918</v>
+        <v>5.491099160457947</v>
       </c>
       <c r="E55" t="n">
-        <v>4.491544144476268</v>
+        <v>6.028534441092638</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.3212600295927115</v>
+        <v>-0.05024738692019959</v>
       </c>
       <c r="C56" t="n">
-        <v>0.5552172644389217</v>
+        <v>-0.8061515589106281</v>
       </c>
       <c r="D56" t="n">
-        <v>0.994925186530334</v>
+        <v>3.914952515144929</v>
       </c>
       <c r="E56" t="n">
-        <v>4.281846589096132</v>
+        <v>4.820816495514122</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.8865897347206304</v>
+        <v>0.04373235801182052</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.1838157293050244</v>
+        <v>0.9887468445740148</v>
       </c>
       <c r="D57" t="n">
-        <v>8.787233118628135</v>
+        <v>-6.286756534679779</v>
       </c>
       <c r="E57" t="n">
-        <v>11.75623988198392</v>
+        <v>-5.468508710957233</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.6531721380884912</v>
+        <v>-0.7816461490835112</v>
       </c>
       <c r="C58" t="n">
-        <v>0.6822715978232767</v>
+        <v>-0.5373797488265586</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.6153164432838363</v>
+        <v>9.613207362226023</v>
       </c>
       <c r="E58" t="n">
-        <v>-3.290819174663213</v>
+        <v>8.875848217634353</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.2911739166171814</v>
+        <v>0.3489123638059199</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.02358126741633448</v>
+        <v>-0.9961025561648085</v>
       </c>
       <c r="D59" t="n">
-        <v>0.8347107240021922</v>
+        <v>6.085058658864094</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.1510867996116643</v>
+        <v>5.81337632782878</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.8408387022146264</v>
+        <v>-0.410408938655779</v>
       </c>
       <c r="C60" t="n">
-        <v>0.6144361729926866</v>
+        <v>0.8899267549835901</v>
       </c>
       <c r="D60" t="n">
-        <v>2.330853658590082</v>
+        <v>-5.313464391461711</v>
       </c>
       <c r="E60" t="n">
-        <v>3.38695197756097</v>
+        <v>-5.022407408432731</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.01833046038693675</v>
+        <v>-0.09998553003201205</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.3400950448808604</v>
+        <v>-0.9200829643188253</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2377090185001667</v>
+        <v>6.086880149984364</v>
       </c>
       <c r="E61" t="n">
-        <v>3.347836702889902</v>
+        <v>6.94402040330422</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.5558736168370315</v>
+        <v>-0.6681144614546948</v>
       </c>
       <c r="C62" t="n">
-        <v>0.220118030136184</v>
+        <v>-0.6702236552330283</v>
       </c>
       <c r="D62" t="n">
-        <v>2.241415650036309</v>
+        <v>9.169022277404208</v>
       </c>
       <c r="E62" t="n">
-        <v>0.7137640618775734</v>
+        <v>8.748006871563792</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.1141280296676594</v>
+        <v>0.03109034975425051</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3538524665383367</v>
+        <v>-0.6077895986804787</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1040406080358445</v>
+        <v>1.447215861509168</v>
       </c>
       <c r="E63" t="n">
-        <v>-0.487857303320522</v>
+        <v>1.284090878497727</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-0.4182151222072439</v>
+        <v>0.867599083945563</v>
       </c>
       <c r="C64" t="n">
-        <v>0.7015466190807482</v>
+        <v>-0.6194375214779975</v>
       </c>
       <c r="D64" t="n">
-        <v>-2.385822860249088</v>
+        <v>6.029687154433175</v>
       </c>
       <c r="E64" t="n">
-        <v>-5.912920618416838</v>
+        <v>5.057631415019693</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.9164734663499645</v>
+        <v>-0.512639490173904</v>
       </c>
       <c r="C65" t="n">
-        <v>0.4027099646799839</v>
+        <v>0.952201833573781</v>
       </c>
       <c r="D65" t="n">
-        <v>10.28450719578423</v>
+        <v>-6.209652083199583</v>
       </c>
       <c r="E65" t="n">
-        <v>6.470890342632702</v>
+        <v>-7.260671477670706</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.8367754395770641</v>
+        <v>-0.7346546415676483</v>
       </c>
       <c r="C66" t="n">
-        <v>0.5946609307302253</v>
+        <v>0.8800097514903817</v>
       </c>
       <c r="D66" t="n">
-        <v>8.664295343519308</v>
+        <v>-3.160330424704705</v>
       </c>
       <c r="E66" t="n">
-        <v>11.25470247513401</v>
+        <v>-2.446423328176782</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.472969162228881</v>
+        <v>-0.1416253569540347</v>
       </c>
       <c r="C67" t="n">
-        <v>0.1492056419323773</v>
+        <v>0.6344097167164238</v>
       </c>
       <c r="D67" t="n">
-        <v>1.752718227670326</v>
+        <v>-2.036329006759169</v>
       </c>
       <c r="E67" t="n">
-        <v>6.076536308724185</v>
+        <v>-0.844699947957138</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-0.150628388143103</v>
+        <v>0.5691869856970477</v>
       </c>
       <c r="C68" t="n">
-        <v>0.2595275205271288</v>
+        <v>-0.3900683707353167</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.1253776551008317</v>
+        <v>2.356185822074873</v>
       </c>
       <c r="E68" t="n">
-        <v>-0.3549525527213048</v>
+        <v>2.29291578757116</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.6437485722749796</v>
+        <v>-0.360483313395686</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.9899570321830848</v>
+        <v>-0.116408874617915</v>
       </c>
       <c r="D69" t="n">
-        <v>7.224508855225449</v>
+        <v>1.515971035039747</v>
       </c>
       <c r="E69" t="n">
-        <v>10.42386412968255</v>
+        <v>2.397702098420981</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.3727770804237134</v>
+        <v>-0.2068103839065802</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.5583272613567158</v>
+        <v>0.2582388078053457</v>
       </c>
       <c r="D70" t="n">
-        <v>1.399701041236695</v>
+        <v>-0.001470591536607031</v>
       </c>
       <c r="E70" t="n">
-        <v>2.552629985170864</v>
+        <v>0.3162725712356428</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-0.2329583222897704</v>
+        <v>-0.8428812681659694</v>
       </c>
       <c r="C71" t="n">
-        <v>0.74009679445266</v>
+        <v>0.4097722597052691</v>
       </c>
       <c r="D71" t="n">
-        <v>-3.260972355247158</v>
+        <v>4.523989079903318</v>
       </c>
       <c r="E71" t="n">
-        <v>-5.317673529556291</v>
+        <v>3.957169468477465</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.6804314039082979</v>
+        <v>-0.5757167772226843</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.5127445048088726</v>
+        <v>0.2719811009160131</v>
       </c>
       <c r="D72" t="n">
-        <v>3.548869358025415</v>
+        <v>2.211181207528838</v>
       </c>
       <c r="E72" t="n">
-        <v>4.701031822332955</v>
+        <v>2.528713131211248</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.03229715021291213</v>
+        <v>-0.7494585620936565</v>
       </c>
       <c r="C73" t="n">
-        <v>0.731526143064702</v>
+        <v>-0.2740772848065063</v>
       </c>
       <c r="D73" t="n">
-        <v>-2.494726255146282</v>
+        <v>6.898614669999626</v>
       </c>
       <c r="E73" t="n">
-        <v>2.408675926851975</v>
+        <v>8.249975068964021</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-0.5368696424622157</v>
+        <v>-0.7906707032352196</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.4080768208178311</v>
+        <v>-0.2148489412417853</v>
       </c>
       <c r="D74" t="n">
-        <v>4.615046115674062</v>
+        <v>7.244336324107699</v>
       </c>
       <c r="E74" t="n">
-        <v>4.500829404463004</v>
+        <v>7.212858600131225</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.4813770061043472</v>
+        <v>-0.235385524127931</v>
       </c>
       <c r="C75" t="n">
-        <v>0.02018009562495093</v>
+        <v>0.8381870035803669</v>
       </c>
       <c r="D75" t="n">
-        <v>2.211807317300972</v>
+        <v>-4.621304864439671</v>
       </c>
       <c r="E75" t="n">
-        <v>7.200035349874138</v>
+        <v>-3.246566759339679</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.02426430526769408</v>
+        <v>0.4083228303969222</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.8851325519512341</v>
+        <v>-0.530852037145662</v>
       </c>
       <c r="D76" t="n">
-        <v>5.020672608684016</v>
+        <v>1.429821934381525</v>
       </c>
       <c r="E76" t="n">
-        <v>-3.33131598492211</v>
+        <v>-0.8719567529628813</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.882414430722714</v>
+        <v>0.2130218259624506</v>
       </c>
       <c r="C77" t="n">
-        <v>-0.4773991792461587</v>
+        <v>-0.4286646445667204</v>
       </c>
       <c r="D77" t="n">
-        <v>10.98644367051225</v>
+        <v>0.4540845211689467</v>
       </c>
       <c r="E77" t="n">
-        <v>13.60674452760015</v>
+        <v>1.176230223318554</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-0.4162932510975448</v>
+        <v>-0.3523713133392519</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.3482172202989602</v>
+        <v>-0.6003562846170483</v>
       </c>
       <c r="D78" t="n">
-        <v>2.85141103866465</v>
+        <v>3.966410538037925</v>
       </c>
       <c r="E78" t="n">
-        <v>3.128925106692528</v>
+        <v>4.042892439331927</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.8548618770611542</v>
+        <v>-0.08546944029576498</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.2441759368587906</v>
+        <v>0.805059952158548</v>
       </c>
       <c r="D79" t="n">
-        <v>6.236615282663437</v>
+        <v>-3.855463481216114</v>
       </c>
       <c r="E79" t="n">
-        <v>5.283352319561907</v>
+        <v>-4.11817940177923</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.1307680696590481</v>
+        <v>0.3129870165701034</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.690284663013123</v>
+        <v>0.6162266104302079</v>
       </c>
       <c r="D80" t="n">
-        <v>3.01507455289252</v>
+        <v>0.6297084828226036</v>
       </c>
       <c r="E80" t="n">
-        <v>3.307616356966716</v>
+        <v>0.7103319753272226</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.448574104763531</v>
+        <v>-0.3970022916852405</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.7972322245099426</v>
+        <v>-0.8966545586090755</v>
       </c>
       <c r="D81" t="n">
-        <v>7.683662210068797</v>
+        <v>8.709290246689983</v>
       </c>
       <c r="E81" t="n">
-        <v>1.347109513458014</v>
+        <v>6.962958605449566</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.1576837020972754</v>
+        <v>0.09765432765707183</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.4309792249420217</v>
+        <v>-0.2293768760010535</v>
       </c>
       <c r="D82" t="n">
-        <v>0.4140447167715064</v>
+        <v>0.03753357502109615</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.2862894869991719</v>
+        <v>-0.1554760688727834</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-0.5345563390011216</v>
+        <v>0.8766616870889488</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.4356048249417459</v>
+        <v>0.2463029357649245</v>
       </c>
       <c r="D83" t="n">
-        <v>4.776972875943464</v>
+        <v>8.994672187259708</v>
       </c>
       <c r="E83" t="n">
-        <v>5.915480633527686</v>
+        <v>9.308440921784781</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.1545129161927135</v>
+        <v>-0.1778487223532979</v>
       </c>
       <c r="C84" t="n">
-        <v>0.2975079762026265</v>
+        <v>0.3780080999849491</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3694040618436209</v>
+        <v>-0.4308582842175855</v>
       </c>
       <c r="E84" t="n">
-        <v>5.081066347220191</v>
+        <v>0.8676592734748166</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.9751016495389067</v>
+        <v>-0.6489246832147</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9397123313601203</v>
+        <v>0.3419859213006673</v>
       </c>
       <c r="D85" t="n">
-        <v>9.43017247466743</v>
+        <v>2.580518135132075</v>
       </c>
       <c r="E85" t="n">
-        <v>7.777879301308769</v>
+        <v>2.125151946702031</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.6106961872839007</v>
+        <v>-0.4564261828284062</v>
       </c>
       <c r="C86" t="n">
-        <v>0.97041784448252</v>
+        <v>0.496860138904935</v>
       </c>
       <c r="D86" t="n">
-        <v>1.092072083722523</v>
+        <v>-0.107319889722285</v>
       </c>
       <c r="E86" t="n">
-        <v>-1.485479960873684</v>
+        <v>-0.8176841694717244</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-0.9694519893125182</v>
+        <v>0.902257186084898</v>
       </c>
       <c r="C87" t="n">
-        <v>0.2161024216153338</v>
+        <v>-0.4015444861114681</v>
       </c>
       <c r="D87" t="n">
-        <v>7.989251738619281</v>
+        <v>6.486306513885524</v>
       </c>
       <c r="E87" t="n">
-        <v>6.389604086549073</v>
+        <v>6.045449245999106</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-0.1661959342046611</v>
+        <v>0.2071208357428747</v>
       </c>
       <c r="C88" t="n">
-        <v>0.03570989755044374</v>
+        <v>-0.9444391419399902</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2255765078691113</v>
+        <v>5.167625508923407</v>
       </c>
       <c r="E88" t="n">
-        <v>3.143962740817944</v>
+        <v>5.971922492468562</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-0.4020942439287158</v>
+        <v>-0.3998854872938349</v>
       </c>
       <c r="C89" t="n">
-        <v>0.6159063837059857</v>
+        <v>0.6184903592151423</v>
       </c>
       <c r="D89" t="n">
-        <v>-1.47606509478711</v>
+        <v>-1.480893587393151</v>
       </c>
       <c r="E89" t="n">
-        <v>-0.4279762888469347</v>
+        <v>-1.192043997990669</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.2575235452878735</v>
+        <v>0.2821960319789987</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.5726214202837854</v>
+        <v>-0.9039072643615189</v>
       </c>
       <c r="D90" t="n">
-        <v>1.122632657360693</v>
+        <v>4.455156981242963</v>
       </c>
       <c r="E90" t="n">
-        <v>-0.5662916476419186</v>
+        <v>3.989695381742087</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-0.329554305516883</v>
+        <v>0.880800526921423</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9371255186569485</v>
+        <v>-0.075220711637487</v>
       </c>
       <c r="D91" t="n">
-        <v>-6.426134037206555</v>
+        <v>7.444672098012065</v>
       </c>
       <c r="E91" t="n">
-        <v>-4.789790203548839</v>
+        <v>7.895642704505017</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.8354150646312166</v>
+        <v>-0.3684650509420335</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.9922445449409951</v>
+        <v>-0.6084255305412447</v>
       </c>
       <c r="D92" t="n">
-        <v>8.976346528420775</v>
+        <v>4.218690973044945</v>
       </c>
       <c r="E92" t="n">
-        <v>9.285838693740342</v>
+        <v>4.303985925504293</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.1123221847283931</v>
+        <v>0.5718845414497569</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.2718743090551714</v>
+        <v>-0.3678313293003173</v>
       </c>
       <c r="D93" t="n">
-        <v>0.08863804537589098</v>
+        <v>2.390685051410808</v>
       </c>
       <c r="E93" t="n">
-        <v>3.176767459017984</v>
+        <v>3.241762658667651</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.3916418449724883</v>
+        <v>0.1399551585543333</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.6208921397497711</v>
+        <v>0.9458700606748958</v>
       </c>
       <c r="D94" t="n">
-        <v>4.636687396291323</v>
+        <v>-4.735491737972323</v>
       </c>
       <c r="E94" t="n">
-        <v>2.398477494489872</v>
+        <v>-5.352334516435144</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.9012698622285396</v>
+        <v>-0.5171715064862068</v>
       </c>
       <c r="C95" t="n">
-        <v>-0.6425139496600929</v>
+        <v>-0.5287080010554528</v>
       </c>
       <c r="D95" t="n">
-        <v>13.3730911734447</v>
+        <v>5.273161407086112</v>
       </c>
       <c r="E95" t="n">
-        <v>12.3284740820075</v>
+        <v>4.985268609992665</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-0.5829317154679232</v>
+        <v>0.5726228193845668</v>
       </c>
       <c r="C96" t="n">
-        <v>0.4018582993134061</v>
+        <v>0.5620212738622112</v>
       </c>
       <c r="D96" t="n">
-        <v>1.516233976777794</v>
+        <v>4.112305966712017</v>
       </c>
       <c r="E96" t="n">
-        <v>0.2661570829199718</v>
+        <v>3.767789170553264</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.2066763606629325</v>
+        <v>0.0873207592687899</v>
       </c>
       <c r="C97" t="n">
-        <v>0.5507726297194706</v>
+        <v>0.8022825111446921</v>
       </c>
       <c r="D97" t="n">
-        <v>0.01914256469364529</v>
+        <v>-2.964853850694925</v>
       </c>
       <c r="E97" t="n">
-        <v>-4.646677836798661</v>
+        <v>-4.250737546387888</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.9493301016047997</v>
+        <v>0.5192225517897264</v>
       </c>
       <c r="C98" t="n">
-        <v>0.5060884398440357</v>
+        <v>0.6614102346080446</v>
       </c>
       <c r="D98" t="n">
-        <v>11.13344122670649</v>
+        <v>2.892845024143381</v>
       </c>
       <c r="E98" t="n">
-        <v>12.07749993398983</v>
+        <v>3.153024284168982</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.4361795379234614</v>
+        <v>0.2864309489174657</v>
       </c>
       <c r="C99" t="n">
-        <v>0.2477876326142636</v>
+        <v>0.8693281329378049</v>
       </c>
       <c r="D99" t="n">
-        <v>2.506655581627259</v>
+        <v>-2.093259159622872</v>
       </c>
       <c r="E99" t="n">
-        <v>3.33892382487864</v>
+        <v>-1.863888958382874</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.270119742220293</v>
+        <v>-0.00874622216217924</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.8880612373663375</v>
+        <v>0.6028787751732372</v>
       </c>
       <c r="D100" t="n">
-        <v>7.078997855937583</v>
+        <v>-1.46898109702692</v>
       </c>
       <c r="E100" t="n">
-        <v>7.095300026513286</v>
+        <v>-1.464488276141444</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-0.6472055290871108</v>
+        <v>0.9112913661424231</v>
       </c>
       <c r="C101" t="n">
-        <v>0.7729322307325841</v>
+        <v>-0.014353061650066</v>
       </c>
       <c r="D101" t="n">
-        <v>-2.011436746667171</v>
+        <v>8.315775742745522</v>
       </c>
       <c r="E101" t="n">
-        <v>-2.759322126468941</v>
+        <v>8.109661161947116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>